<commit_message>
move datapackage e de-para anteriores para data-raw
</commit_message>
<xml_diff>
--- a/de-para-ckan-portal.xlsx
+++ b/de-para-ckan-portal.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$B$1:$E$61</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -207,7 +210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -215,14 +218,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A34" sqref="A33:XFD34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,488 +535,613 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
+      <c r="C7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C12" t="s">
-        <v>23</v>
-      </c>
+      <c r="C12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
+      <c r="C13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C14" t="s">
-        <v>23</v>
-      </c>
+      <c r="C14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C15" t="s">
-        <v>22</v>
-      </c>
+      <c r="C15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="C17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="C18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="C19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="C20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+      <c r="C21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="C22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="C23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="C24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="C25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C26" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+      <c r="C26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C27" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+      <c r="C27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C28" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+      <c r="C28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="1" t="s">
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="1" t="s">
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="1" t="s">
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="1" t="s">
+      <c r="C37" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="1" t="s">
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="1" t="s">
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="1" t="s">
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="1" t="s">
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+      <c r="C42" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>16</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>16</v>
-      </c>
-      <c r="C49" s="1" t="s">
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>16</v>
-      </c>
-      <c r="C50" s="1" t="s">
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>16</v>
-      </c>
-      <c r="C51" s="1" t="s">
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>16</v>
-      </c>
-      <c r="C52" s="1" t="s">
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>16</v>
-      </c>
-      <c r="C53" s="1" t="s">
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>16</v>
-      </c>
-      <c r="C58" t="s">
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B58" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>16</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B59" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>16</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>16</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="B1:E61"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>